<commit_message>
feat(meeting-invitations): add endpoint for uploading meeting invitations via Excel file
</commit_message>
<xml_diff>
--- a/backend/test/Asamblea_Test_Usuarios.xlsx
+++ b/backend/test/Asamblea_Test_Usuarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJECTS\Asambleas\backend\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B781FA93-96D0-4D1D-812C-B46B5175DF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44094F4E-D885-4045-8581-AF6B746E11D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{4B71C7F7-FF66-4ADA-A27D-72916E4A2A49}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{4B71C7F7-FF66-4ADA-A27D-72916E4A2A49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>email</t>
   </si>
@@ -59,56 +59,38 @@
     <t>password</t>
   </si>
   <si>
-    <t>juan.perez@email.com</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Pérez</t>
-  </si>
-  <si>
     <t>0.25</t>
   </si>
   <si>
-    <t>MiPassword123</t>
-  </si>
-  <si>
-    <t>maria.garcia@email.com</t>
-  </si>
-  <si>
-    <t>María</t>
-  </si>
-  <si>
-    <t>García</t>
-  </si>
-  <si>
     <t>0.30</t>
   </si>
   <si>
-    <t>Password456</t>
-  </si>
-  <si>
-    <t>carlos.lopez@email.com</t>
-  </si>
-  <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>López</t>
-  </si>
-  <si>
-    <t>0.45</t>
-  </si>
-  <si>
-    <t>CarlosPass789</t>
+    <t>ramirezvalencias27@gmail.com</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>RamirezV.20</t>
+  </si>
+  <si>
+    <t>santiagorv796@gmail.com</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>RamirezV.21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +102,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,16 +147,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B66A25-AE88-4F8C-8B6D-31809E186FCA}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,73 +533,53 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>3053263366</v>
+      </c>
+      <c r="E2">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3">
-        <v>3001234567</v>
-      </c>
-      <c r="E2" s="3">
-        <v>101</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3">
-        <v>3009876543</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>102</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3">
-        <v>201</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1E9560D1-5107-4B6E-AC13-0368623197F8}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{68C0086B-9674-43E0-BEBA-6F814E2E2D8B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(Administrador): Creación del administrador desde la opción del la asamblea, además de envio de correo con sus respectivas credenciales
</commit_message>
<xml_diff>
--- a/backend/test/Asamblea_Test_Usuarios.xlsx
+++ b/backend/test/Asamblea_Test_Usuarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJECTS\Asambleas\backend\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCODE\AsambleasGiramaster\backend\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44094F4E-D885-4045-8581-AF6B746E11D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A348DD7-4017-4198-B2F2-95DC25151077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{4B71C7F7-FF66-4ADA-A27D-72916E4A2A49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B71C7F7-FF66-4ADA-A27D-72916E4A2A49}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -62,9 +51,6 @@
     <t>0.25</t>
   </si>
   <si>
-    <t>0.30</t>
-  </si>
-  <si>
     <t>ramirezvalencias27@gmail.com</t>
   </si>
   <si>
@@ -75,15 +61,6 @@
   </si>
   <si>
     <t>RamirezV.20</t>
-  </si>
-  <si>
-    <t>santiagorv796@gmail.com</t>
-  </si>
-  <si>
-    <t>Valencia</t>
-  </si>
-  <si>
-    <t>RamirezV.21</t>
   </si>
 </sst>
 </file>
@@ -158,7 +135,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,13 +468,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B66A25-AE88-4F8C-8B6D-31809E186FCA}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -533,13 +510,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2">
         <v>3053263366</v>
@@ -551,35 +528,14 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>102</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{1E9560D1-5107-4B6E-AC13-0368623197F8}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{68C0086B-9674-43E0-BEBA-6F814E2E2D8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
style(ExcelUploadModal): Ajuste visual en el modal para subir el archivo de excel con los copropietarios
</commit_message>
<xml_diff>
--- a/backend/test/Asamblea_Test_Usuarios.xlsx
+++ b/backend/test/Asamblea_Test_Usuarios.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCODE\AsambleasGiramaster\backend\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3098AC64-B608-4606-9F21-3BDFAEE71B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -55,8 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,38 +133,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -170,10 +172,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -211,71 +213,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -303,7 +305,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -326,11 +328,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -339,13 +341,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -355,7 +357,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -364,7 +366,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -373,7 +375,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -381,10 +383,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -449,26 +451,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="18.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,26 +495,26 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>3053263366</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>101</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(super_admin): permitir administradores cargar copropietarios
</commit_message>
<xml_diff>
--- a/backend/test/Asamblea_Test_Usuarios.xlsx
+++ b/backend/test/Asamblea_Test_Usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCODE\AsambleasGiramaster\backend\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3098AC64-B608-4606-9F21-3BDFAEE71B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE0CA4-A3D9-4CFD-A37E-98CA3B370CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>email</t>
   </si>
@@ -40,9 +40,6 @@
     <t>voting_weight</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>santiagorv796@gmail.com</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t>0.25</t>
-  </si>
-  <si>
-    <t>RamirezV.20</t>
   </si>
 </sst>
 </file>
@@ -455,10 +449,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,10 +463,9 @@
     <col min="4" max="4" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,31 +484,25 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="4">
         <v>3053263366</v>
       </c>
       <c r="E2" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(poderes): Actualizar la funcionalidad para ceder el poder en los modales para los copropietarios invitados a la reunión
</commit_message>
<xml_diff>
--- a/backend/test/Asamblea_Test_Usuarios.xlsx
+++ b/backend/test/Asamblea_Test_Usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSCODE\AsambleasGiramaster\backend\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE0CA4-A3D9-4CFD-A37E-98CA3B370CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB48DDF1-B442-4202-890F-A7974811A08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>email</t>
   </si>
@@ -50,13 +50,22 @@
   </si>
   <si>
     <t>0.25</t>
+  </si>
+  <si>
+    <t>ramirezvalencias27@gmail.com</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>0.30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +92,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,10 +141,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -144,8 +162,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,15 +469,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -505,7 +525,30 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3106301469</v>
+      </c>
+      <c r="E3" s="5">
+        <v>202</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{D4A33396-883E-4BAD-9631-11BE93D345B4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>